<commit_message>
Atualização do texto de análise e realizações de algumas análises
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/HVMP x Hibrída 2 com Add-Drop + 2-OPT.xlsx
+++ b/Arquivos/Comparações/HVMP x Hibrída 2 com Add-Drop + 2-OPT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="76">
   <si>
     <t>Instâncias</t>
   </si>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>Resultados positivos para Híbrida2</t>
+  </si>
+  <si>
+    <t>Resultados finais da análise</t>
+  </si>
+  <si>
+    <t>Héuristica + buscas locais</t>
+  </si>
+  <si>
+    <t>Número de vezes que teve o melhor resultado</t>
+  </si>
+  <si>
+    <t>HVMP</t>
+  </si>
+  <si>
+    <t>Híbrida 2</t>
+  </si>
+  <si>
+    <t>Resultados iguais</t>
   </si>
 </sst>
 </file>
@@ -231,13 +249,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="0_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -262,7 +280,60 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -274,9 +345,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,10 +368,41 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -305,106 +414,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,25 +430,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +484,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,43 +580,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -515,91 +610,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,22 +654,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,6 +693,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -711,17 +726,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -730,152 +741,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -891,11 +902,20 @@
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1216,16 +1236,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:R65"/>
+  <dimension ref="B2:R76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="10.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="15.8571428571429" customWidth="1"/>
+    <col min="2" max="2" width="18.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="20.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="26.8571428571429" customWidth="1"/>
     <col min="5" max="5" width="28.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="16.2857142857143" customWidth="1"/>
@@ -4421,24 +4441,75 @@
       <c r="N65" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="O65" s="6"/>
-      <c r="P65" s="6">
+      <c r="O65" s="5"/>
+      <c r="P65" s="5">
         <f>COUNTIF(R3:R64,"HVMP")</f>
         <v>43</v>
       </c>
       <c r="Q65" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="R65" s="6">
+      <c r="R65" s="5">
         <f>COUNTIF(R3:R64,"Híbrida 2")</f>
         <v>19</v>
       </c>
     </row>
+    <row r="70" spans="2:3">
+      <c r="B70" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" ht="26" customHeight="1" spans="2:3">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="8">
+        <f>D65+J65+P65</f>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" s="8">
+        <f>F65+L65+R65</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="B75" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C75" s="8">
+        <f>COUNTIF(F3:F64,"Igual")+COUNTIF(L3:L64,"Igual")+COUNTIF(R3:R64,"Igual")</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="H65:I65"/>
     <mergeCell ref="N65:O65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>